<commit_message>
Add final requests and files
</commit_message>
<xml_diff>
--- a/Endpoints List (Excel).xlsx
+++ b/Endpoints List (Excel).xlsx
@@ -18,7 +18,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="368" uniqueCount="274">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="660" uniqueCount="300">
   <si>
     <t>Endpoint name:</t>
   </si>
@@ -859,10 +859,88 @@
     <t>Link to Trello API - Developer documentation:</t>
   </si>
   <si>
-    <t>This request is misspelled in the documentation</t>
-  </si>
-  <si>
-    <t>Custom Fields Power-Up disabled for board</t>
+    <t>Can't get key. No explanation in the documentation.</t>
+  </si>
+  <si>
+    <t>Technically this request works but I don't know how to fully write it correctly.</t>
+  </si>
+  <si>
+    <t>Enterprise version of Trello is payable.</t>
+  </si>
+  <si>
+    <t>"Feature not enabled"</t>
+  </si>
+  <si>
+    <t>Only for paid Business Class.</t>
+  </si>
+  <si>
+    <t>This request get full name of second member.</t>
+  </si>
+  <si>
+    <t>Request dosen't work.</t>
+  </si>
+  <si>
+    <t>Custom Fields Power-Up disabled for board.</t>
+  </si>
+  <si>
+    <t>This request is misspelled in the documentation.</t>
+  </si>
+  <si>
+    <t>"Unauthorized"</t>
+  </si>
+  <si>
+    <t>Propably doesn't work if invited member haven't trello accound. "Unauthorized"</t>
+  </si>
+  <si>
+    <t>"Unauthorized organization" - I don't know why</t>
+  </si>
+  <si>
+    <t>"Removal feature not enabled"</t>
+  </si>
+  <si>
+    <t>"Expected string but received a undefined." - I don't know why</t>
+  </si>
+  <si>
+    <t>"The requested resource was not found"</t>
+  </si>
+  <si>
+    <t>I can't get idPlugin and use any plugins.</t>
+  </si>
+  <si>
+    <t>Too advanced for simple exercise.</t>
+  </si>
+  <si>
+    <t>Can't get - "The ID of the notification"</t>
+  </si>
+  <si>
+    <t>Can't get - "The ID of the action"</t>
+  </si>
+  <si>
+    <t>Stickers are premium products and not enabled.</t>
+  </si>
+  <si>
+    <t>"Unauthorized card permission requested"</t>
+  </si>
+  <si>
+    <t>Custom Fields Power-Up disabled.</t>
+  </si>
+  <si>
+    <t>Request doesn't work.</t>
+  </si>
+  <si>
+    <t>"Can't generate calendarKey"</t>
+  </si>
+  <si>
+    <t>This request need organization.</t>
+  </si>
+  <si>
+    <t>"message": "Gone" | Expected response to have status code 200 but got 410</t>
+  </si>
+  <si>
+    <t>This not "Power-Up". This is Plugin.</t>
+  </si>
+  <si>
+    <t>Most requests had the following message: "Unauthorized member permission requested." and I don't know why. In general this category would be too much work + playing with the other accounts ect. A waste of time for a simple exercise to check requests work and use Postman tool.</t>
   </si>
 </sst>
 </file>
@@ -964,7 +1042,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="3">
+  <borders count="6">
     <border>
       <left/>
       <right/>
@@ -998,12 +1076,49 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="14">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
@@ -1026,6 +1141,15 @@
     </xf>
     <xf numFmtId="0" fontId="2" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -1331,15 +1455,15 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:XFC302"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C141" sqref="C141"/>
+    <sheetView tabSelected="1" topLeftCell="A39" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="C39" sqref="C39"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="0" defaultRowHeight="15" zeroHeight="1" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="64.28515625" customWidth="1"/>
     <col min="2" max="2" width="19.28515625" customWidth="1"/>
-    <col min="3" max="3" width="69.42578125" customWidth="1"/>
+    <col min="3" max="3" width="71.5703125" customWidth="1"/>
     <col min="4" max="16383" width="9.140625" hidden="1"/>
     <col min="16384" max="16384" width="69.28515625" hidden="1" customWidth="1"/>
   </cols>
@@ -1380,113 +1504,177 @@
       <c r="A5" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="B5" s="1"/>
-      <c r="C5" s="1"/>
+      <c r="B5" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="C5" s="1" t="s">
+        <v>290</v>
+      </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="B6" s="1"/>
-      <c r="C6" s="1"/>
+      <c r="B6" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="C6" s="1" t="s">
+        <v>290</v>
+      </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="B7" s="1"/>
-      <c r="C7" s="1"/>
+      <c r="B7" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="C7" s="1" t="s">
+        <v>290</v>
+      </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="B8" s="1"/>
-      <c r="C8" s="1"/>
+      <c r="B8" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="C8" s="1" t="s">
+        <v>290</v>
+      </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="B9" s="1"/>
-      <c r="C9" s="1"/>
+      <c r="B9" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="C9" s="1" t="s">
+        <v>290</v>
+      </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="B10" s="1"/>
-      <c r="C10" s="1"/>
+      <c r="B10" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="C10" s="1" t="s">
+        <v>290</v>
+      </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="B11" s="1"/>
-      <c r="C11" s="1"/>
+      <c r="B11" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="C11" s="1" t="s">
+        <v>290</v>
+      </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A12" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="B12" s="1"/>
-      <c r="C12" s="1"/>
+      <c r="B12" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="C12" s="1" t="s">
+        <v>290</v>
+      </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A13" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="B13" s="1"/>
-      <c r="C13" s="1"/>
+      <c r="B13" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="C13" s="1" t="s">
+        <v>290</v>
+      </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A14" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="B14" s="1"/>
-      <c r="C14" s="1"/>
+      <c r="B14" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="C14" s="1" t="s">
+        <v>290</v>
+      </c>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A15" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="B15" s="1"/>
-      <c r="C15" s="1"/>
+      <c r="B15" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="C15" s="1" t="s">
+        <v>290</v>
+      </c>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A16" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="B16" s="1"/>
-      <c r="C16" s="1"/>
+      <c r="B16" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="C16" s="1" t="s">
+        <v>290</v>
+      </c>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A17" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="B17" s="1"/>
-      <c r="C17" s="1"/>
+      <c r="B17" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="C17" s="1" t="s">
+        <v>290</v>
+      </c>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A18" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="B18" s="1"/>
-      <c r="C18" s="1"/>
+      <c r="B18" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="C18" s="1" t="s">
+        <v>290</v>
+      </c>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A19" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="B19" s="1"/>
-      <c r="C19" s="1"/>
+      <c r="B19" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="C19" s="1" t="s">
+        <v>290</v>
+      </c>
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A20" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="B20" s="1"/>
-      <c r="C20" s="1"/>
+      <c r="B20" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="C20" s="1" t="s">
+        <v>290</v>
+      </c>
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A21" s="8"/>
@@ -1515,8 +1703,12 @@
       <c r="A24" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="B24" s="1"/>
-      <c r="C24" s="1"/>
+      <c r="B24" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="C24" s="1" t="s">
+        <v>272</v>
+      </c>
     </row>
     <row r="25" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A25" s="8"/>
@@ -1545,8 +1737,12 @@
       <c r="A28" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="B28" s="1"/>
-      <c r="C28" s="1"/>
+      <c r="B28" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="C28" s="1" t="s">
+        <v>273</v>
+      </c>
     </row>
     <row r="29" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A29" s="8"/>
@@ -1620,7 +1816,9 @@
       <c r="A37" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="B37" s="1"/>
+      <c r="B37" s="2" t="s">
+        <v>4</v>
+      </c>
       <c r="C37" s="1"/>
     </row>
     <row r="38" spans="1:3" x14ac:dyDescent="0.25">
@@ -1636,7 +1834,9 @@
       <c r="A39" s="1" t="s">
         <v>34</v>
       </c>
-      <c r="B39" s="1"/>
+      <c r="B39" s="2" t="s">
+        <v>4</v>
+      </c>
       <c r="C39" s="1"/>
     </row>
     <row r="40" spans="1:3" x14ac:dyDescent="0.25">
@@ -1656,7 +1856,7 @@
         <v>3</v>
       </c>
       <c r="C41" s="1" t="s">
-        <v>272</v>
+        <v>280</v>
       </c>
     </row>
     <row r="42" spans="1:3" x14ac:dyDescent="0.25">
@@ -1681,21 +1881,27 @@
       <c r="A44" s="1" t="s">
         <v>39</v>
       </c>
-      <c r="B44" s="1"/>
+      <c r="B44" s="2" t="s">
+        <v>4</v>
+      </c>
       <c r="C44" s="1"/>
     </row>
     <row r="45" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A45" s="1" t="s">
         <v>40</v>
       </c>
-      <c r="B45" s="1"/>
+      <c r="B45" s="2" t="s">
+        <v>4</v>
+      </c>
       <c r="C45" s="1"/>
     </row>
     <row r="46" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A46" s="1" t="s">
         <v>41</v>
       </c>
-      <c r="B46" s="1"/>
+      <c r="B46" s="2" t="s">
+        <v>4</v>
+      </c>
       <c r="C46" s="1"/>
     </row>
     <row r="47" spans="1:3" x14ac:dyDescent="0.25">
@@ -1720,91 +1926,117 @@
       <c r="A49" s="1" t="s">
         <v>44</v>
       </c>
-      <c r="B49" s="1"/>
+      <c r="B49" s="2" t="s">
+        <v>4</v>
+      </c>
       <c r="C49" s="1"/>
     </row>
     <row r="50" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A50" s="1" t="s">
         <v>45</v>
       </c>
-      <c r="B50" s="1"/>
+      <c r="B50" s="2" t="s">
+        <v>4</v>
+      </c>
       <c r="C50" s="1"/>
     </row>
     <row r="51" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A51" s="1" t="s">
         <v>46</v>
       </c>
-      <c r="B51" s="1"/>
+      <c r="B51" s="2" t="s">
+        <v>4</v>
+      </c>
       <c r="C51" s="1"/>
     </row>
     <row r="52" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A52" s="1" t="s">
         <v>47</v>
       </c>
-      <c r="B52" s="1"/>
+      <c r="B52" s="2" t="s">
+        <v>4</v>
+      </c>
       <c r="C52" s="1"/>
     </row>
     <row r="53" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A53" s="1" t="s">
         <v>48</v>
       </c>
-      <c r="B53" s="1"/>
+      <c r="B53" s="2" t="s">
+        <v>4</v>
+      </c>
       <c r="C53" s="1"/>
     </row>
     <row r="54" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A54" s="1" t="s">
         <v>49</v>
       </c>
-      <c r="B54" s="1"/>
+      <c r="B54" s="2" t="s">
+        <v>4</v>
+      </c>
       <c r="C54" s="1"/>
     </row>
     <row r="55" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A55" s="1" t="s">
         <v>50</v>
       </c>
-      <c r="B55" s="1"/>
+      <c r="B55" s="2" t="s">
+        <v>4</v>
+      </c>
       <c r="C55" s="1"/>
     </row>
     <row r="56" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A56" s="1" t="s">
         <v>51</v>
       </c>
-      <c r="B56" s="1"/>
+      <c r="B56" s="2" t="s">
+        <v>4</v>
+      </c>
       <c r="C56" s="1"/>
     </row>
     <row r="57" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A57" s="1" t="s">
         <v>52</v>
       </c>
-      <c r="B57" s="1"/>
+      <c r="B57" s="2" t="s">
+        <v>4</v>
+      </c>
       <c r="C57" s="1"/>
     </row>
     <row r="58" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A58" s="1" t="s">
         <v>53</v>
       </c>
-      <c r="B58" s="1"/>
+      <c r="B58" s="2" t="s">
+        <v>4</v>
+      </c>
       <c r="C58" s="1"/>
     </row>
     <row r="59" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A59" s="1" t="s">
         <v>54</v>
       </c>
-      <c r="B59" s="1"/>
+      <c r="B59" s="2" t="s">
+        <v>4</v>
+      </c>
       <c r="C59" s="1"/>
     </row>
     <row r="60" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A60" s="1" t="s">
         <v>55</v>
       </c>
-      <c r="B60" s="1"/>
+      <c r="B60" s="2" t="s">
+        <v>4</v>
+      </c>
       <c r="C60" s="1"/>
     </row>
     <row r="61" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A61" s="1" t="s">
         <v>56</v>
       </c>
-      <c r="B61" s="1"/>
+      <c r="B61" s="2" t="s">
+        <v>4</v>
+      </c>
       <c r="C61" s="1"/>
     </row>
     <row r="62" spans="1:3" x14ac:dyDescent="0.25">
@@ -1820,71 +2052,107 @@
       <c r="A63" s="1" t="s">
         <v>58</v>
       </c>
-      <c r="B63" s="1"/>
-      <c r="C63" s="1"/>
+      <c r="B63" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="C63" s="1" t="s">
+        <v>295</v>
+      </c>
     </row>
     <row r="64" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A64" s="1" t="s">
         <v>59</v>
       </c>
-      <c r="B64" s="1"/>
+      <c r="B64" s="2" t="s">
+        <v>4</v>
+      </c>
       <c r="C64" s="1"/>
     </row>
     <row r="65" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A65" s="1" t="s">
         <v>60</v>
       </c>
-      <c r="B65" s="1"/>
-      <c r="C65" s="1"/>
+      <c r="B65" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="C65" s="1" t="s">
+        <v>296</v>
+      </c>
     </row>
     <row r="66" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A66" s="1" t="s">
         <v>61</v>
       </c>
-      <c r="B66" s="1"/>
-      <c r="C66" s="1"/>
+      <c r="B66" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="C66" s="1" t="s">
+        <v>294</v>
+      </c>
     </row>
     <row r="67" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A67" s="1" t="s">
         <v>62</v>
       </c>
-      <c r="B67" s="1"/>
-      <c r="C67" s="1"/>
+      <c r="B67" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="C67" s="1" t="s">
+        <v>297</v>
+      </c>
     </row>
     <row r="68" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A68" s="1" t="s">
         <v>63</v>
       </c>
-      <c r="B68" s="1"/>
+      <c r="B68" s="2" t="s">
+        <v>4</v>
+      </c>
       <c r="C68" s="1"/>
     </row>
     <row r="69" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A69" s="1" t="s">
         <v>64</v>
       </c>
-      <c r="B69" s="1"/>
-      <c r="C69" s="1"/>
+      <c r="B69" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="C69" s="1" t="s">
+        <v>298</v>
+      </c>
     </row>
     <row r="70" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A70" s="1" t="s">
         <v>65</v>
       </c>
-      <c r="B70" s="1"/>
-      <c r="C70" s="1"/>
+      <c r="B70" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="C70" s="1" t="s">
+        <v>298</v>
+      </c>
     </row>
     <row r="71" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A71" s="1" t="s">
         <v>66</v>
       </c>
-      <c r="B71" s="1"/>
-      <c r="C71" s="1"/>
+      <c r="B71" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="C71" s="1" t="s">
+        <v>298</v>
+      </c>
     </row>
     <row r="72" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A72" s="1" t="s">
         <v>67</v>
       </c>
-      <c r="B72" s="1"/>
-      <c r="C72" s="1"/>
+      <c r="B72" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="C72" s="1" t="s">
+        <v>298</v>
+      </c>
     </row>
     <row r="73" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A73" s="8"/>
@@ -1922,280 +2190,372 @@
       <c r="A77" s="1" t="s">
         <v>70</v>
       </c>
-      <c r="B77" s="1"/>
+      <c r="B77" s="2" t="s">
+        <v>4</v>
+      </c>
       <c r="C77" s="1"/>
     </row>
     <row r="78" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A78" s="1" t="s">
         <v>71</v>
       </c>
-      <c r="B78" s="1"/>
+      <c r="B78" s="2" t="s">
+        <v>4</v>
+      </c>
       <c r="C78" s="1"/>
     </row>
     <row r="79" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A79" s="1" t="s">
         <v>72</v>
       </c>
-      <c r="B79" s="1"/>
+      <c r="B79" s="2" t="s">
+        <v>4</v>
+      </c>
       <c r="C79" s="1"/>
     </row>
     <row r="80" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A80" s="1" t="s">
         <v>73</v>
       </c>
-      <c r="B80" s="1"/>
+      <c r="B80" s="2" t="s">
+        <v>4</v>
+      </c>
       <c r="C80" s="1"/>
     </row>
     <row r="81" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A81" s="1" t="s">
         <v>74</v>
       </c>
-      <c r="B81" s="1"/>
+      <c r="B81" s="2" t="s">
+        <v>4</v>
+      </c>
       <c r="C81" s="1"/>
     </row>
     <row r="82" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A82" s="1" t="s">
         <v>75</v>
       </c>
-      <c r="B82" s="1"/>
+      <c r="B82" s="2" t="s">
+        <v>4</v>
+      </c>
       <c r="C82" s="1"/>
     </row>
     <row r="83" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A83" s="1" t="s">
         <v>76</v>
       </c>
-      <c r="B83" s="1"/>
+      <c r="B83" s="2" t="s">
+        <v>4</v>
+      </c>
       <c r="C83" s="1"/>
     </row>
     <row r="84" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A84" s="1" t="s">
         <v>77</v>
       </c>
-      <c r="B84" s="1"/>
+      <c r="B84" s="2" t="s">
+        <v>4</v>
+      </c>
       <c r="C84" s="1"/>
     </row>
     <row r="85" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A85" s="1" t="s">
         <v>78</v>
       </c>
-      <c r="B85" s="1"/>
+      <c r="B85" s="2" t="s">
+        <v>4</v>
+      </c>
       <c r="C85" s="1"/>
     </row>
     <row r="86" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A86" s="1" t="s">
         <v>79</v>
       </c>
-      <c r="B86" s="1"/>
+      <c r="B86" s="2" t="s">
+        <v>4</v>
+      </c>
       <c r="C86" s="1"/>
     </row>
     <row r="87" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A87" s="1" t="s">
         <v>80</v>
       </c>
-      <c r="B87" s="1"/>
+      <c r="B87" s="2" t="s">
+        <v>4</v>
+      </c>
       <c r="C87" s="1"/>
     </row>
     <row r="88" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A88" s="1" t="s">
         <v>81</v>
       </c>
-      <c r="B88" s="1"/>
+      <c r="B88" s="2" t="s">
+        <v>4</v>
+      </c>
       <c r="C88" s="1"/>
     </row>
     <row r="89" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A89" s="1" t="s">
         <v>82</v>
       </c>
-      <c r="B89" s="1"/>
+      <c r="B89" s="2" t="s">
+        <v>4</v>
+      </c>
       <c r="C89" s="1"/>
     </row>
     <row r="90" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A90" s="1" t="s">
         <v>83</v>
       </c>
-      <c r="B90" s="1"/>
+      <c r="B90" s="2" t="s">
+        <v>4</v>
+      </c>
       <c r="C90" s="1"/>
     </row>
     <row r="91" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A91" s="1" t="s">
         <v>84</v>
       </c>
-      <c r="B91" s="1"/>
+      <c r="B91" s="2" t="s">
+        <v>4</v>
+      </c>
       <c r="C91" s="1"/>
     </row>
     <row r="92" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A92" s="1" t="s">
         <v>85</v>
       </c>
-      <c r="B92" s="1"/>
+      <c r="B92" s="2" t="s">
+        <v>4</v>
+      </c>
       <c r="C92" s="1"/>
     </row>
     <row r="93" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A93" s="1" t="s">
         <v>86</v>
       </c>
-      <c r="B93" s="1"/>
+      <c r="B93" s="2" t="s">
+        <v>4</v>
+      </c>
       <c r="C93" s="1"/>
     </row>
     <row r="94" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A94" s="1" t="s">
         <v>87</v>
       </c>
-      <c r="B94" s="1"/>
+      <c r="B94" s="2" t="s">
+        <v>4</v>
+      </c>
       <c r="C94" s="1"/>
     </row>
     <row r="95" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A95" s="1" t="s">
         <v>88</v>
       </c>
-      <c r="B95" s="1"/>
+      <c r="B95" s="2" t="s">
+        <v>4</v>
+      </c>
       <c r="C95" s="1"/>
     </row>
     <row r="96" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A96" s="1" t="s">
         <v>89</v>
       </c>
-      <c r="B96" s="1"/>
-      <c r="C96" s="1"/>
+      <c r="B96" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="C96" s="1" t="s">
+        <v>292</v>
+      </c>
     </row>
     <row r="97" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A97" s="1" t="s">
         <v>90</v>
       </c>
-      <c r="B97" s="1"/>
+      <c r="B97" s="2" t="s">
+        <v>4</v>
+      </c>
       <c r="C97" s="1"/>
     </row>
     <row r="98" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A98" s="1" t="s">
         <v>91</v>
       </c>
-      <c r="B98" s="1"/>
+      <c r="B98" s="2" t="s">
+        <v>4</v>
+      </c>
       <c r="C98" s="1"/>
     </row>
     <row r="99" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A99" s="1" t="s">
         <v>92</v>
       </c>
-      <c r="B99" s="1"/>
-      <c r="C99" s="1"/>
+      <c r="B99" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="C99" s="1" t="s">
+        <v>291</v>
+      </c>
     </row>
     <row r="100" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A100" s="1" t="s">
         <v>93</v>
       </c>
-      <c r="B100" s="1"/>
-      <c r="C100" s="1"/>
+      <c r="B100" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="C100" s="1" t="s">
+        <v>291</v>
+      </c>
     </row>
     <row r="101" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A101" s="1" t="s">
         <v>94</v>
       </c>
-      <c r="B101" s="1"/>
-      <c r="C101" s="1"/>
+      <c r="B101" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="C101" s="1" t="s">
+        <v>291</v>
+      </c>
     </row>
     <row r="102" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A102" s="1" t="s">
         <v>95</v>
       </c>
-      <c r="B102" s="1"/>
-      <c r="C102" s="1"/>
+      <c r="B102" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="C102" s="1" t="s">
+        <v>291</v>
+      </c>
     </row>
     <row r="103" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A103" s="1" t="s">
         <v>96</v>
       </c>
-      <c r="B103" s="1"/>
+      <c r="B103" s="2" t="s">
+        <v>4</v>
+      </c>
       <c r="C103" s="1"/>
     </row>
     <row r="104" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A104" s="1" t="s">
         <v>97</v>
       </c>
-      <c r="B104" s="1"/>
+      <c r="B104" s="2" t="s">
+        <v>4</v>
+      </c>
       <c r="C104" s="1"/>
     </row>
     <row r="105" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A105" s="1" t="s">
         <v>98</v>
       </c>
-      <c r="B105" s="1"/>
-      <c r="C105" s="1"/>
+      <c r="B105" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="C105" s="1" t="s">
+        <v>293</v>
+      </c>
     </row>
     <row r="106" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A106" s="1" t="s">
         <v>99</v>
       </c>
-      <c r="B106" s="1"/>
+      <c r="B106" s="2" t="s">
+        <v>4</v>
+      </c>
       <c r="C106" s="1"/>
     </row>
     <row r="107" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A107" s="1" t="s">
         <v>100</v>
       </c>
-      <c r="B107" s="1"/>
+      <c r="B107" s="2" t="s">
+        <v>4</v>
+      </c>
       <c r="C107" s="1"/>
     </row>
     <row r="108" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A108" s="1" t="s">
         <v>101</v>
       </c>
-      <c r="B108" s="1"/>
+      <c r="B108" s="2" t="s">
+        <v>4</v>
+      </c>
       <c r="C108" s="1"/>
     </row>
     <row r="109" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A109" s="1" t="s">
         <v>102</v>
       </c>
-      <c r="B109" s="1"/>
+      <c r="B109" s="2" t="s">
+        <v>4</v>
+      </c>
       <c r="C109" s="1"/>
     </row>
     <row r="110" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A110" s="1" t="s">
         <v>103</v>
       </c>
-      <c r="B110" s="1"/>
+      <c r="B110" s="2" t="s">
+        <v>4</v>
+      </c>
       <c r="C110" s="1"/>
     </row>
     <row r="111" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A111" s="1" t="s">
         <v>104</v>
       </c>
-      <c r="B111" s="1"/>
+      <c r="B111" s="2" t="s">
+        <v>4</v>
+      </c>
       <c r="C111" s="1"/>
     </row>
     <row r="112" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A112" s="1" t="s">
         <v>105</v>
       </c>
-      <c r="B112" s="1"/>
+      <c r="B112" s="2" t="s">
+        <v>4</v>
+      </c>
       <c r="C112" s="1"/>
     </row>
     <row r="113" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A113" s="1" t="s">
         <v>106</v>
       </c>
-      <c r="B113" s="1"/>
+      <c r="B113" s="2" t="s">
+        <v>4</v>
+      </c>
       <c r="C113" s="1"/>
     </row>
     <row r="114" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A114" s="1" t="s">
         <v>107</v>
       </c>
-      <c r="B114" s="1"/>
+      <c r="B114" s="3" t="s">
+        <v>3</v>
+      </c>
       <c r="C114" s="1"/>
     </row>
     <row r="115" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A115" s="1" t="s">
         <v>108</v>
       </c>
-      <c r="B115" s="1"/>
+      <c r="B115" s="2" t="s">
+        <v>4</v>
+      </c>
       <c r="C115" s="1"/>
     </row>
     <row r="116" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A116" s="1" t="s">
         <v>109</v>
       </c>
-      <c r="B116" s="1"/>
+      <c r="B116" s="2" t="s">
+        <v>4</v>
+      </c>
       <c r="C116" s="1"/>
     </row>
     <row r="117" spans="1:3" x14ac:dyDescent="0.25">
@@ -2234,77 +2594,99 @@
       <c r="A121" s="1" t="s">
         <v>112</v>
       </c>
-      <c r="B121" s="1"/>
+      <c r="B121" s="2" t="s">
+        <v>4</v>
+      </c>
       <c r="C121" s="1"/>
     </row>
     <row r="122" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A122" s="1" t="s">
         <v>113</v>
       </c>
-      <c r="B122" s="1"/>
+      <c r="B122" s="2" t="s">
+        <v>4</v>
+      </c>
       <c r="C122" s="1"/>
     </row>
     <row r="123" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A123" s="1" t="s">
         <v>114</v>
       </c>
-      <c r="B123" s="1"/>
+      <c r="B123" s="2" t="s">
+        <v>4</v>
+      </c>
       <c r="C123" s="1"/>
     </row>
     <row r="124" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A124" s="1" t="s">
         <v>115</v>
       </c>
-      <c r="B124" s="1"/>
+      <c r="B124" s="2" t="s">
+        <v>4</v>
+      </c>
       <c r="C124" s="1"/>
     </row>
     <row r="125" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A125" s="1" t="s">
         <v>116</v>
       </c>
-      <c r="B125" s="1"/>
+      <c r="B125" s="2" t="s">
+        <v>4</v>
+      </c>
       <c r="C125" s="1"/>
     </row>
     <row r="126" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A126" s="1" t="s">
         <v>117</v>
       </c>
-      <c r="B126" s="1"/>
+      <c r="B126" s="2" t="s">
+        <v>4</v>
+      </c>
       <c r="C126" s="1"/>
     </row>
     <row r="127" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A127" s="1" t="s">
         <v>118</v>
       </c>
-      <c r="B127" s="1"/>
+      <c r="B127" s="2" t="s">
+        <v>4</v>
+      </c>
       <c r="C127" s="1"/>
     </row>
     <row r="128" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A128" s="1" t="s">
         <v>119</v>
       </c>
-      <c r="B128" s="1"/>
+      <c r="B128" s="2" t="s">
+        <v>4</v>
+      </c>
       <c r="C128" s="1"/>
     </row>
     <row r="129" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A129" s="1" t="s">
         <v>120</v>
       </c>
-      <c r="B129" s="1"/>
+      <c r="B129" s="2" t="s">
+        <v>4</v>
+      </c>
       <c r="C129" s="1"/>
     </row>
     <row r="130" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A130" s="1" t="s">
         <v>121</v>
       </c>
-      <c r="B130" s="1"/>
+      <c r="B130" s="2" t="s">
+        <v>4</v>
+      </c>
       <c r="C130" s="1"/>
     </row>
     <row r="131" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A131" s="1" t="s">
         <v>122</v>
       </c>
-      <c r="B131" s="1"/>
+      <c r="B131" s="2" t="s">
+        <v>4</v>
+      </c>
       <c r="C131" s="1"/>
     </row>
     <row r="132" spans="1:3" x14ac:dyDescent="0.25">
@@ -2338,7 +2720,7 @@
         <v>3</v>
       </c>
       <c r="C135" s="1" t="s">
-        <v>273</v>
+        <v>279</v>
       </c>
     </row>
     <row r="136" spans="1:3" x14ac:dyDescent="0.25">
@@ -2349,7 +2731,7 @@
         <v>3</v>
       </c>
       <c r="C136" s="1" t="s">
-        <v>273</v>
+        <v>279</v>
       </c>
     </row>
     <row r="137" spans="1:3" x14ac:dyDescent="0.25">
@@ -2360,7 +2742,7 @@
         <v>3</v>
       </c>
       <c r="C137" s="1" t="s">
-        <v>273</v>
+        <v>279</v>
       </c>
     </row>
     <row r="138" spans="1:3" x14ac:dyDescent="0.25">
@@ -2371,7 +2753,7 @@
         <v>3</v>
       </c>
       <c r="C138" s="1" t="s">
-        <v>273</v>
+        <v>279</v>
       </c>
     </row>
     <row r="139" spans="1:3" x14ac:dyDescent="0.25">
@@ -2382,7 +2764,7 @@
         <v>3</v>
       </c>
       <c r="C139" s="1" t="s">
-        <v>273</v>
+        <v>279</v>
       </c>
     </row>
     <row r="140" spans="1:3" x14ac:dyDescent="0.25">
@@ -2393,7 +2775,7 @@
         <v>3</v>
       </c>
       <c r="C140" s="1" t="s">
-        <v>273</v>
+        <v>279</v>
       </c>
     </row>
     <row r="141" spans="1:3" x14ac:dyDescent="0.25">
@@ -2404,7 +2786,7 @@
         <v>3</v>
       </c>
       <c r="C141" s="1" t="s">
-        <v>273</v>
+        <v>279</v>
       </c>
     </row>
     <row r="142" spans="1:3" x14ac:dyDescent="0.25">
@@ -2415,7 +2797,7 @@
         <v>3</v>
       </c>
       <c r="C142" s="1" t="s">
-        <v>273</v>
+        <v>279</v>
       </c>
     </row>
     <row r="143" spans="1:3" x14ac:dyDescent="0.25">
@@ -2477,85 +2859,133 @@
       <c r="A150" s="1" t="s">
         <v>135</v>
       </c>
-      <c r="B150" s="1"/>
-      <c r="C150" s="1"/>
+      <c r="B150" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="C150" s="1" t="s">
+        <v>274</v>
+      </c>
     </row>
     <row r="151" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A151" s="1" t="s">
         <v>136</v>
       </c>
-      <c r="B151" s="1"/>
-      <c r="C151" s="1"/>
+      <c r="B151" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="C151" s="1" t="s">
+        <v>274</v>
+      </c>
     </row>
     <row r="152" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A152" s="1" t="s">
         <v>137</v>
       </c>
-      <c r="B152" s="1"/>
-      <c r="C152" s="1"/>
+      <c r="B152" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="C152" s="1" t="s">
+        <v>274</v>
+      </c>
     </row>
     <row r="153" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A153" s="1" t="s">
         <v>138</v>
       </c>
-      <c r="B153" s="1"/>
-      <c r="C153" s="1"/>
+      <c r="B153" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="C153" s="1" t="s">
+        <v>274</v>
+      </c>
     </row>
     <row r="154" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A154" s="1" t="s">
         <v>139</v>
       </c>
-      <c r="B154" s="1"/>
-      <c r="C154" s="1"/>
+      <c r="B154" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="C154" s="1" t="s">
+        <v>274</v>
+      </c>
     </row>
     <row r="155" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A155" s="1" t="s">
         <v>140</v>
       </c>
-      <c r="B155" s="1"/>
-      <c r="C155" s="1"/>
+      <c r="B155" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="C155" s="1" t="s">
+        <v>274</v>
+      </c>
     </row>
     <row r="156" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A156" s="1" t="s">
         <v>141</v>
       </c>
-      <c r="B156" s="1"/>
-      <c r="C156" s="1"/>
+      <c r="B156" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="C156" s="1" t="s">
+        <v>274</v>
+      </c>
     </row>
     <row r="157" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A157" s="1" t="s">
         <v>142</v>
       </c>
-      <c r="B157" s="1"/>
-      <c r="C157" s="1"/>
+      <c r="B157" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="C157" s="1" t="s">
+        <v>274</v>
+      </c>
     </row>
     <row r="158" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A158" s="1" t="s">
         <v>143</v>
       </c>
-      <c r="B158" s="1"/>
-      <c r="C158" s="1"/>
+      <c r="B158" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="C158" s="1" t="s">
+        <v>274</v>
+      </c>
     </row>
     <row r="159" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A159" s="1" t="s">
         <v>144</v>
       </c>
-      <c r="B159" s="1"/>
-      <c r="C159" s="1"/>
+      <c r="B159" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="C159" s="1" t="s">
+        <v>274</v>
+      </c>
     </row>
     <row r="160" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A160" s="1" t="s">
         <v>145</v>
       </c>
-      <c r="B160" s="1"/>
-      <c r="C160" s="1"/>
+      <c r="B160" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="C160" s="1" t="s">
+        <v>274</v>
+      </c>
     </row>
     <row r="161" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A161" s="1" t="s">
         <v>146</v>
       </c>
-      <c r="B161" s="1"/>
-      <c r="C161" s="1"/>
+      <c r="B161" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="C161" s="1" t="s">
+        <v>274</v>
+      </c>
     </row>
     <row r="162" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A162" s="8"/>
@@ -2652,77 +3082,99 @@
       <c r="A173" s="1" t="s">
         <v>154</v>
       </c>
-      <c r="B173" s="1"/>
+      <c r="B173" s="2" t="s">
+        <v>4</v>
+      </c>
       <c r="C173" s="1"/>
     </row>
     <row r="174" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A174" s="1" t="s">
         <v>155</v>
       </c>
-      <c r="B174" s="1"/>
+      <c r="B174" s="2" t="s">
+        <v>4</v>
+      </c>
       <c r="C174" s="1"/>
     </row>
     <row r="175" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A175" s="1" t="s">
         <v>156</v>
       </c>
-      <c r="B175" s="1"/>
+      <c r="B175" s="2" t="s">
+        <v>4</v>
+      </c>
       <c r="C175" s="1"/>
     </row>
     <row r="176" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A176" s="1" t="s">
         <v>157</v>
       </c>
-      <c r="B176" s="1"/>
+      <c r="B176" s="2" t="s">
+        <v>4</v>
+      </c>
       <c r="C176" s="1"/>
     </row>
     <row r="177" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A177" s="1" t="s">
         <v>158</v>
       </c>
-      <c r="B177" s="1"/>
+      <c r="B177" s="2" t="s">
+        <v>4</v>
+      </c>
       <c r="C177" s="1"/>
     </row>
     <row r="178" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A178" s="1" t="s">
         <v>159</v>
       </c>
-      <c r="B178" s="1"/>
+      <c r="B178" s="2" t="s">
+        <v>4</v>
+      </c>
       <c r="C178" s="1"/>
     </row>
     <row r="179" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A179" s="1" t="s">
         <v>160</v>
       </c>
-      <c r="B179" s="1"/>
+      <c r="B179" s="2" t="s">
+        <v>4</v>
+      </c>
       <c r="C179" s="1"/>
     </row>
     <row r="180" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A180" s="1" t="s">
         <v>161</v>
       </c>
-      <c r="B180" s="1"/>
+      <c r="B180" s="2" t="s">
+        <v>4</v>
+      </c>
       <c r="C180" s="1"/>
     </row>
     <row r="181" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A181" s="1" t="s">
         <v>162</v>
       </c>
-      <c r="B181" s="1"/>
+      <c r="B181" s="2" t="s">
+        <v>4</v>
+      </c>
       <c r="C181" s="1"/>
     </row>
     <row r="182" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A182" s="1" t="s">
         <v>163</v>
       </c>
-      <c r="B182" s="1"/>
+      <c r="B182" s="2" t="s">
+        <v>4</v>
+      </c>
       <c r="C182" s="1"/>
     </row>
     <row r="183" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A183" s="1" t="s">
         <v>164</v>
       </c>
-      <c r="B183" s="1"/>
+      <c r="B183" s="2" t="s">
+        <v>4</v>
+      </c>
       <c r="C183" s="1"/>
     </row>
     <row r="184" spans="1:3" x14ac:dyDescent="0.25">
@@ -2752,281 +3204,363 @@
       <c r="A187" s="1" t="s">
         <v>166</v>
       </c>
-      <c r="B187" s="1"/>
-      <c r="C187" s="1"/>
+      <c r="B187" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="C187" s="11" t="s">
+        <v>299</v>
+      </c>
     </row>
     <row r="188" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A188" s="1" t="s">
         <v>167</v>
       </c>
-      <c r="B188" s="1"/>
-      <c r="C188" s="1"/>
+      <c r="B188" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="C188" s="12"/>
     </row>
     <row r="189" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A189" s="1" t="s">
         <v>168</v>
       </c>
-      <c r="B189" s="1"/>
-      <c r="C189" s="1"/>
+      <c r="B189" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="C189" s="12"/>
     </row>
     <row r="190" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A190" s="1" t="s">
         <v>169</v>
       </c>
-      <c r="B190" s="1"/>
-      <c r="C190" s="1"/>
+      <c r="B190" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="C190" s="12"/>
     </row>
     <row r="191" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A191" s="1" t="s">
         <v>170</v>
       </c>
-      <c r="B191" s="1"/>
-      <c r="C191" s="1"/>
+      <c r="B191" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="C191" s="12"/>
     </row>
     <row r="192" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A192" s="1" t="s">
         <v>171</v>
       </c>
-      <c r="B192" s="1"/>
-      <c r="C192" s="1"/>
+      <c r="B192" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="C192" s="12"/>
     </row>
     <row r="193" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A193" s="1" t="s">
         <v>172</v>
       </c>
-      <c r="B193" s="1"/>
-      <c r="C193" s="1"/>
+      <c r="B193" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="C193" s="12"/>
     </row>
     <row r="194" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A194" s="1" t="s">
         <v>173</v>
       </c>
-      <c r="B194" s="1"/>
-      <c r="C194" s="1"/>
+      <c r="B194" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="C194" s="12"/>
     </row>
     <row r="195" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A195" s="1" t="s">
         <v>174</v>
       </c>
-      <c r="B195" s="1"/>
-      <c r="C195" s="1"/>
+      <c r="B195" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="C195" s="12"/>
     </row>
     <row r="196" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A196" s="1" t="s">
         <v>175</v>
       </c>
-      <c r="B196" s="1"/>
-      <c r="C196" s="1"/>
+      <c r="B196" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="C196" s="12"/>
     </row>
     <row r="197" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A197" s="1" t="s">
         <v>176</v>
       </c>
-      <c r="B197" s="1"/>
-      <c r="C197" s="1"/>
+      <c r="B197" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="C197" s="12"/>
     </row>
     <row r="198" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A198" s="1" t="s">
         <v>177</v>
       </c>
-      <c r="B198" s="1"/>
-      <c r="C198" s="1"/>
+      <c r="B198" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="C198" s="12"/>
     </row>
     <row r="199" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A199" s="1" t="s">
         <v>178</v>
       </c>
-      <c r="B199" s="1"/>
-      <c r="C199" s="1"/>
+      <c r="B199" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="C199" s="12"/>
     </row>
     <row r="200" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A200" s="1" t="s">
         <v>179</v>
       </c>
-      <c r="B200" s="1"/>
-      <c r="C200" s="1"/>
+      <c r="B200" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="C200" s="12"/>
     </row>
     <row r="201" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A201" s="1" t="s">
         <v>180</v>
       </c>
-      <c r="B201" s="1"/>
-      <c r="C201" s="1"/>
+      <c r="B201" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="C201" s="12"/>
     </row>
     <row r="202" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A202" s="1" t="s">
         <v>181</v>
       </c>
-      <c r="B202" s="1"/>
-      <c r="C202" s="1"/>
+      <c r="B202" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="C202" s="12"/>
     </row>
     <row r="203" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A203" s="1" t="s">
         <v>182</v>
       </c>
-      <c r="B203" s="1"/>
-      <c r="C203" s="1"/>
+      <c r="B203" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="C203" s="12"/>
     </row>
     <row r="204" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A204" s="1" t="s">
         <v>183</v>
       </c>
-      <c r="B204" s="1"/>
-      <c r="C204" s="1"/>
+      <c r="B204" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="C204" s="12"/>
     </row>
     <row r="205" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A205" s="1" t="s">
         <v>184</v>
       </c>
-      <c r="B205" s="1"/>
-      <c r="C205" s="1"/>
+      <c r="B205" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="C205" s="12"/>
     </row>
     <row r="206" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A206" s="1" t="s">
         <v>185</v>
       </c>
-      <c r="B206" s="1"/>
-      <c r="C206" s="1"/>
+      <c r="B206" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="C206" s="12"/>
     </row>
     <row r="207" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A207" s="1" t="s">
         <v>186</v>
       </c>
-      <c r="B207" s="1"/>
-      <c r="C207" s="1"/>
+      <c r="B207" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="C207" s="12"/>
     </row>
     <row r="208" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A208" s="1" t="s">
         <v>187</v>
       </c>
-      <c r="B208" s="1"/>
-      <c r="C208" s="1"/>
+      <c r="B208" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="C208" s="12"/>
     </row>
     <row r="209" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A209" s="1" t="s">
         <v>188</v>
       </c>
-      <c r="B209" s="1"/>
-      <c r="C209" s="1"/>
+      <c r="B209" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="C209" s="12"/>
     </row>
     <row r="210" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A210" s="1" t="s">
         <v>189</v>
       </c>
-      <c r="B210" s="1"/>
-      <c r="C210" s="1"/>
+      <c r="B210" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="C210" s="12"/>
     </row>
     <row r="211" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A211" s="1" t="s">
         <v>190</v>
       </c>
-      <c r="B211" s="1"/>
-      <c r="C211" s="1"/>
+      <c r="B211" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="C211" s="12"/>
     </row>
     <row r="212" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A212" s="1" t="s">
         <v>191</v>
       </c>
-      <c r="B212" s="1"/>
-      <c r="C212" s="1"/>
+      <c r="B212" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="C212" s="12"/>
     </row>
     <row r="213" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A213" s="1" t="s">
         <v>192</v>
       </c>
-      <c r="B213" s="1"/>
-      <c r="C213" s="1"/>
+      <c r="B213" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="C213" s="12"/>
     </row>
     <row r="214" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A214" s="1" t="s">
         <v>193</v>
       </c>
-      <c r="B214" s="1"/>
-      <c r="C214" s="1"/>
+      <c r="B214" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="C214" s="12"/>
     </row>
     <row r="215" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A215" s="1" t="s">
         <v>194</v>
       </c>
-      <c r="B215" s="1"/>
-      <c r="C215" s="1"/>
+      <c r="B215" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="C215" s="12"/>
     </row>
     <row r="216" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A216" s="1" t="s">
         <v>195</v>
       </c>
-      <c r="B216" s="1"/>
-      <c r="C216" s="1"/>
+      <c r="B216" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="C216" s="12"/>
     </row>
     <row r="217" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A217" s="1" t="s">
         <v>196</v>
       </c>
-      <c r="B217" s="1"/>
-      <c r="C217" s="1"/>
+      <c r="B217" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="C217" s="12"/>
     </row>
     <row r="218" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A218" s="1" t="s">
         <v>197</v>
       </c>
-      <c r="B218" s="1"/>
-      <c r="C218" s="1"/>
+      <c r="B218" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="C218" s="12"/>
     </row>
     <row r="219" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A219" s="1" t="s">
         <v>198</v>
       </c>
-      <c r="B219" s="1"/>
-      <c r="C219" s="1"/>
+      <c r="B219" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="C219" s="12"/>
     </row>
     <row r="220" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A220" s="1" t="s">
         <v>199</v>
       </c>
-      <c r="B220" s="1"/>
-      <c r="C220" s="1"/>
+      <c r="B220" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="C220" s="12"/>
     </row>
     <row r="221" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A221" s="1" t="s">
         <v>200</v>
       </c>
-      <c r="B221" s="1"/>
-      <c r="C221" s="1"/>
+      <c r="B221" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="C221" s="12"/>
     </row>
     <row r="222" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A222" s="1" t="s">
         <v>201</v>
       </c>
-      <c r="B222" s="1"/>
-      <c r="C222" s="1"/>
+      <c r="B222" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="C222" s="12"/>
     </row>
     <row r="223" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A223" s="1" t="s">
         <v>202</v>
       </c>
-      <c r="B223" s="1"/>
-      <c r="C223" s="1"/>
+      <c r="B223" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="C223" s="12"/>
     </row>
     <row r="224" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A224" s="1" t="s">
         <v>203</v>
       </c>
-      <c r="B224" s="1"/>
-      <c r="C224" s="1"/>
+      <c r="B224" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="C224" s="12"/>
     </row>
     <row r="225" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A225" s="1" t="s">
         <v>204</v>
       </c>
-      <c r="B225" s="1"/>
-      <c r="C225" s="1"/>
+      <c r="B225" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="C225" s="12"/>
     </row>
     <row r="226" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A226" s="1" t="s">
         <v>205</v>
       </c>
-      <c r="B226" s="1"/>
-      <c r="C226" s="1"/>
+      <c r="B226" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="C226" s="13"/>
     </row>
     <row r="227" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A227" s="8"/>
@@ -3055,78 +3589,122 @@
       <c r="A230" s="1" t="s">
         <v>207</v>
       </c>
-      <c r="B230" s="1"/>
-      <c r="C230" s="1"/>
+      <c r="B230" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="C230" s="1" t="s">
+        <v>289</v>
+      </c>
     </row>
     <row r="231" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A231" s="1" t="s">
         <v>208</v>
       </c>
-      <c r="B231" s="1"/>
-      <c r="C231" s="1"/>
+      <c r="B231" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="C231" s="1" t="s">
+        <v>289</v>
+      </c>
     </row>
     <row r="232" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A232" s="1" t="s">
         <v>209</v>
       </c>
-      <c r="B232" s="1"/>
-      <c r="C232" s="1"/>
+      <c r="B232" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="C232" s="1" t="s">
+        <v>289</v>
+      </c>
     </row>
     <row r="233" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A233" s="1" t="s">
         <v>210</v>
       </c>
-      <c r="B233" s="1"/>
-      <c r="C233" s="1"/>
+      <c r="B233" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="C233" s="1" t="s">
+        <v>289</v>
+      </c>
     </row>
     <row r="234" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A234" s="1" t="s">
         <v>211</v>
       </c>
-      <c r="B234" s="1"/>
-      <c r="C234" s="1"/>
+      <c r="B234" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="C234" s="1" t="s">
+        <v>289</v>
+      </c>
     </row>
     <row r="235" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A235" s="1" t="s">
         <v>212</v>
       </c>
-      <c r="B235" s="1"/>
-      <c r="C235" s="1"/>
+      <c r="B235" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="C235" s="1" t="s">
+        <v>289</v>
+      </c>
     </row>
     <row r="236" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A236" s="1" t="s">
         <v>213</v>
       </c>
-      <c r="B236" s="1"/>
-      <c r="C236" s="1"/>
+      <c r="B236" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="C236" s="1" t="s">
+        <v>289</v>
+      </c>
     </row>
     <row r="237" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A237" s="1" t="s">
         <v>214</v>
       </c>
-      <c r="B237" s="1"/>
-      <c r="C237" s="1"/>
+      <c r="B237" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="C237" s="1" t="s">
+        <v>289</v>
+      </c>
     </row>
     <row r="238" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A238" s="1" t="s">
         <v>215</v>
       </c>
-      <c r="B238" s="1"/>
-      <c r="C238" s="1"/>
+      <c r="B238" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="C238" s="1" t="s">
+        <v>289</v>
+      </c>
     </row>
     <row r="239" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A239" s="1" t="s">
         <v>216</v>
       </c>
-      <c r="B239" s="1"/>
-      <c r="C239" s="1"/>
+      <c r="B239" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="C239" s="1" t="s">
+        <v>289</v>
+      </c>
     </row>
     <row r="240" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A240" s="1" t="s">
         <v>217</v>
       </c>
-      <c r="B240" s="1"/>
-      <c r="C240" s="1"/>
+      <c r="B240" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="C240" s="1" t="s">
+        <v>289</v>
+      </c>
     </row>
     <row r="241" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A241" s="8"/>
@@ -3155,189 +3733,267 @@
       <c r="A244" s="1" t="s">
         <v>219</v>
       </c>
-      <c r="B244" s="1"/>
+      <c r="B244" s="2" t="s">
+        <v>4</v>
+      </c>
       <c r="C244" s="1"/>
     </row>
     <row r="245" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A245" s="1" t="s">
         <v>220</v>
       </c>
-      <c r="B245" s="1"/>
+      <c r="B245" s="2" t="s">
+        <v>4</v>
+      </c>
       <c r="C245" s="1"/>
     </row>
     <row r="246" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A246" s="1" t="s">
         <v>221</v>
       </c>
-      <c r="B246" s="1"/>
+      <c r="B246" s="2" t="s">
+        <v>4</v>
+      </c>
       <c r="C246" s="1"/>
     </row>
     <row r="247" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A247" s="1" t="s">
         <v>222</v>
       </c>
-      <c r="B247" s="1"/>
+      <c r="B247" s="2" t="s">
+        <v>4</v>
+      </c>
       <c r="C247" s="1"/>
     </row>
     <row r="248" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A248" s="1" t="s">
         <v>223</v>
       </c>
-      <c r="B248" s="1"/>
+      <c r="B248" s="2" t="s">
+        <v>4</v>
+      </c>
       <c r="C248" s="1"/>
     </row>
     <row r="249" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A249" s="1" t="s">
         <v>224</v>
       </c>
-      <c r="B249" s="1"/>
+      <c r="B249" s="2" t="s">
+        <v>4</v>
+      </c>
       <c r="C249" s="1"/>
     </row>
     <row r="250" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A250" s="1" t="s">
         <v>225</v>
       </c>
-      <c r="B250" s="1"/>
+      <c r="B250" s="2" t="s">
+        <v>4</v>
+      </c>
       <c r="C250" s="1"/>
     </row>
     <row r="251" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A251" s="1" t="s">
         <v>226</v>
       </c>
-      <c r="B251" s="1"/>
-      <c r="C251" s="1"/>
+      <c r="B251" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="C251" s="1" t="s">
+        <v>276</v>
+      </c>
     </row>
     <row r="252" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A252" s="1" t="s">
         <v>227</v>
       </c>
-      <c r="B252" s="1"/>
-      <c r="C252" s="1"/>
+      <c r="B252" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="C252" s="1" t="s">
+        <v>276</v>
+      </c>
     </row>
     <row r="253" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A253" s="1" t="s">
         <v>228</v>
       </c>
-      <c r="B253" s="1"/>
-      <c r="C253" s="1"/>
+      <c r="B253" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="C253" s="1" t="s">
+        <v>277</v>
+      </c>
     </row>
     <row r="254" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A254" s="1" t="s">
         <v>229</v>
       </c>
-      <c r="B254" s="1"/>
-      <c r="C254" s="1"/>
+      <c r="B254" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="C254" s="1" t="s">
+        <v>282</v>
+      </c>
     </row>
     <row r="255" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A255" s="1" t="s">
         <v>230</v>
       </c>
-      <c r="B255" s="1"/>
-      <c r="C255" s="1"/>
+      <c r="B255" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="C255" s="1" t="s">
+        <v>278</v>
+      </c>
     </row>
     <row r="256" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A256" s="1" t="s">
         <v>231</v>
       </c>
-      <c r="B256" s="1"/>
+      <c r="B256" s="2" t="s">
+        <v>4</v>
+      </c>
       <c r="C256" s="1"/>
     </row>
     <row r="257" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A257" s="1" t="s">
         <v>232</v>
       </c>
-      <c r="B257" s="1"/>
+      <c r="B257" s="2" t="s">
+        <v>4</v>
+      </c>
       <c r="C257" s="1"/>
     </row>
     <row r="258" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A258" s="1" t="s">
         <v>233</v>
       </c>
-      <c r="B258" s="1"/>
+      <c r="B258" s="2" t="s">
+        <v>4</v>
+      </c>
       <c r="C258" s="1"/>
     </row>
     <row r="259" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A259" s="1" t="s">
         <v>234</v>
       </c>
-      <c r="B259" s="1"/>
+      <c r="B259" s="2" t="s">
+        <v>4</v>
+      </c>
       <c r="C259" s="1"/>
     </row>
     <row r="260" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A260" s="1" t="s">
         <v>235</v>
       </c>
-      <c r="B260" s="1"/>
-      <c r="C260" s="1"/>
+      <c r="B260" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="C260" s="1" t="s">
+        <v>275</v>
+      </c>
     </row>
     <row r="261" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A261" s="1" t="s">
         <v>236</v>
       </c>
-      <c r="B261" s="1"/>
-      <c r="C261" s="1"/>
+      <c r="B261" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="C261" s="1" t="s">
+        <v>281</v>
+      </c>
     </row>
     <row r="262" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A262" s="1" t="s">
         <v>237</v>
       </c>
-      <c r="B262" s="1"/>
+      <c r="B262" s="2" t="s">
+        <v>4</v>
+      </c>
       <c r="C262" s="1"/>
     </row>
     <row r="263" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A263" s="1" t="s">
         <v>238</v>
       </c>
-      <c r="B263" s="1"/>
-      <c r="C263" s="1"/>
+      <c r="B263" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="C263" s="1" t="s">
+        <v>283</v>
+      </c>
     </row>
     <row r="264" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A264" s="1" t="s">
         <v>239</v>
       </c>
-      <c r="B264" s="1"/>
+      <c r="B264" s="2" t="s">
+        <v>4</v>
+      </c>
       <c r="C264" s="1"/>
     </row>
     <row r="265" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A265" s="1" t="s">
         <v>240</v>
       </c>
-      <c r="B265" s="1"/>
+      <c r="B265" s="2" t="s">
+        <v>4</v>
+      </c>
       <c r="C265" s="1"/>
     </row>
     <row r="266" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A266" s="1" t="s">
         <v>241</v>
       </c>
-      <c r="B266" s="1"/>
-      <c r="C266" s="1"/>
+      <c r="B266" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="C266" s="1" t="s">
+        <v>284</v>
+      </c>
     </row>
     <row r="267" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A267" s="1" t="s">
         <v>242</v>
       </c>
-      <c r="B267" s="1"/>
-      <c r="C267" s="1"/>
+      <c r="B267" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="C267" s="1" t="s">
+        <v>283</v>
+      </c>
     </row>
     <row r="268" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A268" s="1" t="s">
         <v>243</v>
       </c>
-      <c r="B268" s="1"/>
-      <c r="C268" s="1"/>
+      <c r="B268" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="C268" s="1" t="s">
+        <v>285</v>
+      </c>
     </row>
     <row r="269" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A269" s="1" t="s">
         <v>244</v>
       </c>
-      <c r="B269" s="1"/>
-      <c r="C269" s="1"/>
+      <c r="B269" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="C269" s="1" t="s">
+        <v>275</v>
+      </c>
     </row>
     <row r="270" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A270" s="1" t="s">
         <v>245</v>
       </c>
-      <c r="B270" s="1"/>
+      <c r="B270" s="2" t="s">
+        <v>4</v>
+      </c>
       <c r="C270" s="1"/>
     </row>
     <row r="271" spans="1:3" x14ac:dyDescent="0.25">
@@ -3367,36 +4023,56 @@
       <c r="A274" s="1" t="s">
         <v>247</v>
       </c>
-      <c r="B274" s="1"/>
-      <c r="C274" s="1"/>
+      <c r="B274" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="C274" s="1" t="s">
+        <v>286</v>
+      </c>
     </row>
     <row r="275" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A275" s="1" t="s">
         <v>248</v>
       </c>
-      <c r="B275" s="1"/>
-      <c r="C275" s="1"/>
+      <c r="B275" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="C275" s="1" t="s">
+        <v>287</v>
+      </c>
     </row>
     <row r="276" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A276" s="1" t="s">
         <v>249</v>
       </c>
-      <c r="B276" s="1"/>
-      <c r="C276" s="1"/>
+      <c r="B276" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="C276" s="1" t="s">
+        <v>287</v>
+      </c>
     </row>
     <row r="277" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A277" s="1" t="s">
         <v>250</v>
       </c>
-      <c r="B277" s="1"/>
-      <c r="C277" s="1"/>
+      <c r="B277" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="C277" s="1" t="s">
+        <v>287</v>
+      </c>
     </row>
     <row r="278" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A278" s="1" t="s">
         <v>251</v>
       </c>
-      <c r="B278" s="1"/>
-      <c r="C278" s="1"/>
+      <c r="B278" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="C278" s="1" t="s">
+        <v>287</v>
+      </c>
     </row>
     <row r="279" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A279" s="8"/>
@@ -3466,57 +4142,89 @@
       <c r="A287" s="1" t="s">
         <v>256</v>
       </c>
-      <c r="B287" s="1"/>
-      <c r="C287" s="1"/>
+      <c r="B287" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="C287" s="1" t="s">
+        <v>288</v>
+      </c>
     </row>
     <row r="288" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A288" s="1" t="s">
         <v>257</v>
       </c>
-      <c r="B288" s="1"/>
-      <c r="C288" s="1"/>
+      <c r="B288" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="C288" s="1" t="s">
+        <v>288</v>
+      </c>
     </row>
     <row r="289" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A289" s="1" t="s">
         <v>258</v>
       </c>
-      <c r="B289" s="1"/>
-      <c r="C289" s="1"/>
+      <c r="B289" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="C289" s="1" t="s">
+        <v>288</v>
+      </c>
     </row>
     <row r="290" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A290" s="1" t="s">
         <v>259</v>
       </c>
-      <c r="B290" s="1"/>
-      <c r="C290" s="1"/>
+      <c r="B290" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="C290" s="1" t="s">
+        <v>288</v>
+      </c>
     </row>
     <row r="291" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A291" s="1" t="s">
         <v>260</v>
       </c>
-      <c r="B291" s="1"/>
-      <c r="C291" s="1"/>
+      <c r="B291" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="C291" s="1" t="s">
+        <v>288</v>
+      </c>
     </row>
     <row r="292" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A292" s="1" t="s">
         <v>261</v>
       </c>
-      <c r="B292" s="1"/>
-      <c r="C292" s="1"/>
+      <c r="B292" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="C292" s="1" t="s">
+        <v>288</v>
+      </c>
     </row>
     <row r="293" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A293" s="1" t="s">
         <v>262</v>
       </c>
-      <c r="B293" s="1"/>
-      <c r="C293" s="1"/>
+      <c r="B293" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="C293" s="1" t="s">
+        <v>288</v>
+      </c>
     </row>
     <row r="294" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A294" s="1" t="s">
         <v>263</v>
       </c>
-      <c r="B294" s="1"/>
-      <c r="C294" s="1"/>
+      <c r="B294" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="C294" s="1" t="s">
+        <v>288</v>
+      </c>
     </row>
     <row r="295" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A295" s="8"/>
@@ -3587,7 +4295,8 @@
       <c r="C302" s="1"/>
     </row>
   </sheetData>
-  <mergeCells count="37">
+  <mergeCells count="38">
+    <mergeCell ref="C187:C226"/>
     <mergeCell ref="A285:C285"/>
     <mergeCell ref="A118:C118"/>
     <mergeCell ref="A2:C2"/>
@@ -3630,7 +4339,10 @@
     <hyperlink ref="C1" r:id="rId1"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" scale="57" orientation="portrait" r:id="rId2"/>
+  <pageSetup paperSize="9" scale="56" orientation="portrait" r:id="rId2"/>
+  <colBreaks count="1" manualBreakCount="1">
+    <brk id="3" max="301" man="1"/>
+  </colBreaks>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
       <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="1">
@@ -3638,7 +4350,7 @@
           <x14:formula1>
             <xm:f>'Sheet cell data'!$A$1:$A$3</xm:f>
           </x14:formula1>
-          <xm:sqref>B5:B20 B24 B28 B165:B169 B32:B72 B76:B116 B120:B131 B282:B283 B150:B161 B146 B173:B183 B187:B226 B230:B240 B244:B270 B274:B278 B298:B302 B287:B294 B135:B142</xm:sqref>
+          <xm:sqref>B230:B240 B173:B183 B24 B165:B169 B76:B116 B5:B20 B28 B282:B283 B150:B161 B146 B135:B142 B32:B72 B287:B294 B120:B131 B244:B270 B298:B302 B274:B278 B187:B226</xm:sqref>
         </x14:dataValidation>
       </x14:dataValidations>
     </ext>

</xml_diff>